<commit_message>
Optimize code #3 + regex
</commit_message>
<xml_diff>
--- a/Orinoco/Plan_de_test.xlsx
+++ b/Orinoco/Plan_de_test.xlsx
@@ -305,14 +305,14 @@
     <t>collectContactdetails</t>
   </si>
   <si>
-    <t>151 à 174</t>
-  </si>
-  <si>
     <t>La fonction doit afficher la page confirmation de commande</t>
   </si>
   <si>
     <t>Vérifier que la page "Orinoco - commande" s'affiche, 
 sinon une alerte s'affiche : "L'envoi de la commande a échouée"</t>
+  </si>
+  <si>
+    <t>152 à 175</t>
   </si>
 </sst>
 </file>
@@ -645,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,48 +1007,48 @@
         <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>